<commit_message>
about to make data2 global variable
</commit_message>
<xml_diff>
--- a/data/data_chartTwo.xlsx
+++ b/data/data_chartTwo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Country name</t>
   </si>
@@ -201,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +379,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -542,9 +548,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:K49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1402,10 @@
       <c r="C15" s="1">
         <v>1.2809999999999999</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2">
+        <f>(D17-D14)/3+D14</f>
+        <v>8.4529999999999994</v>
+      </c>
       <c r="E15" s="1">
         <v>0.22800000000000001</v>
       </c>
@@ -1405,7 +1415,10 @@
       <c r="G15" s="1">
         <v>0.36799999999999999</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="2">
+        <f>(H17-H14)/3+H14</f>
+        <v>4.3333333333333321E-2</v>
+      </c>
       <c r="I15" s="1">
         <v>0.73299999999999998</v>
       </c>
@@ -1426,7 +1439,10 @@
       <c r="C16" s="1">
         <v>1.446</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2">
+        <f>(D17-D14)*2/3+D14</f>
+        <v>9.5809999999999995</v>
+      </c>
       <c r="E16" s="1">
         <v>0.36799999999999999</v>
       </c>
@@ -1436,7 +1452,10 @@
       <c r="G16" s="1">
         <v>0.22800000000000001</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="2">
+        <f>(H17-H14)*2/3+H14</f>
+        <v>0.17166666666666663</v>
+      </c>
       <c r="I16" s="1">
         <v>0.73799999999999999</v>
       </c>
@@ -1452,32 +1471,34 @@
         <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="C17" s="1">
-        <v>7.3410000000000002</v>
+        <v>7.2539999999999996</v>
       </c>
       <c r="D17" s="1">
-        <v>10.662000000000001</v>
+        <v>10.709</v>
       </c>
       <c r="E17" s="1">
-        <v>0.96799999999999997</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="F17" s="1">
-        <v>69.8</v>
+        <v>70.040000000000006</v>
       </c>
       <c r="G17" s="1">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="H17" s="1"/>
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.3</v>
+      </c>
       <c r="I17" s="1">
-        <v>0.39</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="J17" s="1">
-        <v>0.77</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="K17" s="1">
-        <v>0.23799999999999999</v>
+        <v>0.218</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1485,34 +1506,34 @@
         <v>12</v>
       </c>
       <c r="B18" s="1">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="C18" s="1">
-        <v>7.2850000000000001</v>
+        <v>7.45</v>
       </c>
       <c r="D18" s="1">
-        <v>10.694000000000001</v>
+        <v>10.714</v>
       </c>
       <c r="E18" s="1">
-        <v>0.96499999999999997</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="F18" s="1">
-        <v>69.959999999999994</v>
+        <v>70.2</v>
       </c>
       <c r="G18" s="1">
-        <v>0.89100000000000001</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="H18" s="1">
-        <v>0.34200000000000003</v>
+        <v>0.311</v>
       </c>
       <c r="I18" s="1">
-        <v>0.51300000000000001</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="J18" s="1">
         <v>0.76200000000000001</v>
       </c>
       <c r="K18" s="1">
-        <v>0.215</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1520,34 +1541,34 @@
         <v>12</v>
       </c>
       <c r="B19" s="1">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="C19" s="1">
-        <v>7.2539999999999996</v>
+        <v>7.4059999999999997</v>
       </c>
       <c r="D19" s="1">
-        <v>10.709</v>
+        <v>10.723000000000001</v>
       </c>
       <c r="E19" s="1">
-        <v>0.94699999999999995</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="F19" s="1">
-        <v>70.040000000000006</v>
+        <v>70.28</v>
       </c>
       <c r="G19" s="1">
-        <v>0.91600000000000004</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="H19" s="1">
-        <v>0.3</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="I19" s="1">
-        <v>0.43099999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="J19" s="1">
-        <v>0.72899999999999998</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="K19" s="1">
-        <v>0.218</v>
+        <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1555,34 +1576,34 @@
         <v>12</v>
       </c>
       <c r="B20" s="1">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="C20" s="1">
-        <v>7.45</v>
+        <v>7.1959999999999997</v>
       </c>
       <c r="D20" s="1">
-        <v>10.714</v>
+        <v>10.744</v>
       </c>
       <c r="E20" s="1">
-        <v>0.95499999999999996</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="F20" s="1">
-        <v>70.2</v>
+        <v>70.36</v>
       </c>
       <c r="G20" s="1">
-        <v>0.93200000000000005</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="H20" s="1">
-        <v>0.311</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="I20" s="1">
-        <v>0.36599999999999999</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="J20" s="1">
-        <v>0.76200000000000001</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="K20" s="1">
-        <v>0.22</v>
+        <v>0.214</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1590,34 +1611,34 @@
         <v>12</v>
       </c>
       <c r="B21" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="C21" s="1">
-        <v>7.4059999999999997</v>
+        <v>7.3639999999999999</v>
       </c>
       <c r="D21" s="1">
-        <v>10.723000000000001</v>
+        <v>10.752000000000001</v>
       </c>
       <c r="E21" s="1">
-        <v>0.96699999999999997</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="F21" s="1">
-        <v>70.28</v>
+        <v>70.44</v>
       </c>
       <c r="G21" s="1">
-        <v>0.94499999999999995</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="H21" s="1">
-        <v>0.36399999999999999</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="I21" s="1">
-        <v>0.38200000000000001</v>
+        <v>0.432</v>
       </c>
       <c r="J21" s="1">
-        <v>0.72399999999999998</v>
+        <v>0.77</v>
       </c>
       <c r="K21" s="1">
-        <v>0.19500000000000001</v>
+        <v>0.17699999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1625,34 +1646,34 @@
         <v>12</v>
       </c>
       <c r="B22" s="1">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="C22" s="1">
-        <v>7.1959999999999997</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="D22" s="1">
-        <v>10.744</v>
+        <v>10.763</v>
       </c>
       <c r="E22" s="1">
-        <v>0.94499999999999995</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="F22" s="1">
-        <v>70.36</v>
+        <v>70.52</v>
       </c>
       <c r="G22" s="1">
-        <v>0.93500000000000005</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="H22" s="1">
-        <v>0.26800000000000002</v>
+        <v>0.313</v>
       </c>
       <c r="I22" s="1">
-        <v>0.36799999999999999</v>
+        <v>0.442</v>
       </c>
       <c r="J22" s="1">
-        <v>0.72799999999999998</v>
+        <v>0.74</v>
       </c>
       <c r="K22" s="1">
-        <v>0.214</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1660,34 +1681,34 @@
         <v>12</v>
       </c>
       <c r="B23" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="C23" s="1">
-        <v>7.3639999999999999</v>
+        <v>7.3090000000000002</v>
       </c>
       <c r="D23" s="1">
-        <v>10.752000000000001</v>
+        <v>10.77</v>
       </c>
       <c r="E23" s="1">
-        <v>0.92800000000000005</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="F23" s="1">
-        <v>70.44</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="G23" s="1">
-        <v>0.93300000000000005</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="H23" s="1">
-        <v>0.26300000000000001</v>
+        <v>0.32700000000000001</v>
       </c>
       <c r="I23" s="1">
-        <v>0.432</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J23" s="1">
-        <v>0.77</v>
+        <v>0.75</v>
       </c>
       <c r="K23" s="1">
-        <v>0.17699999999999999</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1695,34 +1716,34 @@
         <v>12</v>
       </c>
       <c r="B24" s="1">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C24" s="1">
-        <v>7.2889999999999997</v>
+        <v>7.25</v>
       </c>
       <c r="D24" s="1">
-        <v>10.763</v>
+        <v>10.781000000000001</v>
       </c>
       <c r="E24" s="1">
-        <v>0.92400000000000004</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="F24" s="1">
-        <v>70.52</v>
+        <v>70.674999999999997</v>
       </c>
       <c r="G24" s="1">
-        <v>0.92300000000000004</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="H24" s="1">
-        <v>0.313</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="I24" s="1">
-        <v>0.442</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="J24" s="1">
-        <v>0.74</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="K24" s="1">
-        <v>0.245</v>
+        <v>0.23599999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1730,34 +1751,34 @@
         <v>12</v>
       </c>
       <c r="B25" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="C25" s="1">
-        <v>7.3090000000000002</v>
+        <v>7.2569999999999997</v>
       </c>
       <c r="D25" s="1">
-        <v>10.77</v>
+        <v>10.787000000000001</v>
       </c>
       <c r="E25" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.95</v>
       </c>
       <c r="F25" s="1">
-        <v>70.599999999999994</v>
+        <v>70.75</v>
       </c>
       <c r="G25" s="1">
-        <v>0.92200000000000004</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="H25" s="1">
-        <v>0.32700000000000001</v>
+        <v>0.312</v>
       </c>
       <c r="I25" s="1">
-        <v>0.35699999999999998</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="J25" s="1">
-        <v>0.75</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="K25" s="1">
-        <v>0.21</v>
+        <v>0.22500000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1765,34 +1786,34 @@
         <v>12</v>
       </c>
       <c r="B26" s="1">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="C26" s="1">
-        <v>7.25</v>
+        <v>7.1769999999999996</v>
       </c>
       <c r="D26" s="1">
-        <v>10.781000000000001</v>
+        <v>10.801</v>
       </c>
       <c r="E26" s="1">
-        <v>0.94199999999999995</v>
+        <v>0.94</v>
       </c>
       <c r="F26" s="1">
-        <v>70.674999999999997</v>
+        <v>70.825000000000003</v>
       </c>
       <c r="G26" s="1">
-        <v>0.92200000000000004</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="H26" s="1">
-        <v>0.23300000000000001</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="I26" s="1">
-        <v>0.39900000000000002</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="J26" s="1">
-        <v>0.73599999999999999</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="K26" s="1">
-        <v>0.23599999999999999</v>
+        <v>0.187</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1800,34 +1821,34 @@
         <v>12</v>
       </c>
       <c r="B27" s="1">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="C27" s="1">
-        <v>7.2569999999999997</v>
+        <v>7.234</v>
       </c>
       <c r="D27" s="1">
-        <v>10.787000000000001</v>
+        <v>10.807</v>
       </c>
       <c r="E27" s="1">
-        <v>0.95</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="F27" s="1">
-        <v>70.75</v>
+        <v>70.900000000000006</v>
       </c>
       <c r="G27" s="1">
-        <v>0.91100000000000003</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="H27" s="1">
-        <v>0.312</v>
+        <v>0.115</v>
       </c>
       <c r="I27" s="1">
-        <v>0.41099999999999998</v>
+        <v>0.43</v>
       </c>
       <c r="J27" s="1">
-        <v>0.72799999999999998</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="K27" s="1">
-        <v>0.22500000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1835,34 +1856,34 @@
         <v>12</v>
       </c>
       <c r="B28" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C28" s="1">
-        <v>7.1769999999999996</v>
+        <v>7.1369999999999996</v>
       </c>
       <c r="D28" s="1">
-        <v>10.801</v>
+        <v>10.794</v>
       </c>
       <c r="E28" s="1">
-        <v>0.94</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="F28" s="1">
-        <v>70.825000000000003</v>
+        <v>70.974999999999994</v>
       </c>
       <c r="G28" s="1">
-        <v>0.91600000000000004</v>
+        <v>0.90500000000000003</v>
       </c>
       <c r="H28" s="1">
-        <v>0.14099999999999999</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I28" s="1">
-        <v>0.40500000000000003</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="J28" s="1">
-        <v>0.70599999999999996</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="K28" s="1">
-        <v>0.187</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1870,34 +1891,34 @@
         <v>12</v>
       </c>
       <c r="B29" s="1">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="C29" s="1">
-        <v>7.234</v>
+        <v>7.1120000000000001</v>
       </c>
       <c r="D29" s="1">
-        <v>10.807</v>
+        <v>10.815</v>
       </c>
       <c r="E29" s="1">
-        <v>0.94299999999999995</v>
+        <v>0.92</v>
       </c>
       <c r="F29" s="1">
-        <v>70.900000000000006</v>
+        <v>71.05</v>
       </c>
       <c r="G29" s="1">
-        <v>0.91800000000000004</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="H29" s="1">
-        <v>0.115</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="I29" s="1">
-        <v>0.43</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="J29" s="1">
-        <v>0.72699999999999998</v>
+        <v>0.74</v>
       </c>
       <c r="K29" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.23499999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1905,34 +1926,34 @@
         <v>12</v>
       </c>
       <c r="B30" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="C30" s="1">
-        <v>7.1369999999999996</v>
+        <v>7.0350000000000001</v>
       </c>
       <c r="D30" s="1">
-        <v>10.794</v>
+        <v>10.84</v>
       </c>
       <c r="E30" s="1">
-        <v>0.93700000000000006</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="F30" s="1">
-        <v>70.974999999999994</v>
+        <v>71.125</v>
       </c>
       <c r="G30" s="1">
-        <v>0.90500000000000003</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="H30" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.153</v>
       </c>
       <c r="I30" s="1">
-        <v>0.49099999999999999</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="J30" s="1">
-        <v>0.72599999999999998</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="K30" s="1">
-        <v>0.20499999999999999</v>
+        <v>0.24399999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1940,104 +1961,104 @@
         <v>12</v>
       </c>
       <c r="B31" s="1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C31" s="1">
-        <v>7.1120000000000001</v>
+        <v>7.0250000000000004</v>
       </c>
       <c r="D31" s="1">
-        <v>10.815</v>
+        <v>10.846</v>
       </c>
       <c r="E31" s="1">
-        <v>0.92</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="F31" s="1">
-        <v>71.05</v>
+        <v>71.2</v>
       </c>
       <c r="G31" s="1">
-        <v>0.91200000000000003</v>
+        <v>0.876</v>
       </c>
       <c r="H31" s="1">
-        <v>0.23400000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="I31" s="1">
-        <v>0.45400000000000001</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="J31" s="1">
-        <v>0.74</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="K31" s="1">
-        <v>0.23499999999999999</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="1">
-        <v>2022</v>
+        <v>2008</v>
       </c>
       <c r="C32" s="1">
-        <v>7.0350000000000001</v>
+        <v>7.6710000000000003</v>
       </c>
       <c r="D32" s="1">
-        <v>10.84</v>
+        <v>10.795999999999999</v>
       </c>
       <c r="E32" s="1">
-        <v>0.94199999999999995</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="F32" s="1">
-        <v>71.125</v>
+        <v>69.16</v>
       </c>
       <c r="G32" s="1">
-        <v>0.85399999999999998</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="H32" s="1">
-        <v>0.153</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>0.54500000000000004</v>
+        <v>0.217</v>
       </c>
       <c r="J32" s="1">
-        <v>0.71099999999999997</v>
+        <v>0.69099999999999995</v>
       </c>
       <c r="K32" s="1">
-        <v>0.24399999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" s="1">
-        <v>2023</v>
+        <v>2010</v>
       </c>
       <c r="C33" s="1">
-        <v>7.0250000000000004</v>
+        <v>7.3929999999999998</v>
       </c>
       <c r="D33" s="1">
-        <v>10.846</v>
+        <v>10.734</v>
       </c>
       <c r="E33" s="1">
-        <v>0.89600000000000002</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="F33" s="1">
-        <v>71.2</v>
+        <v>69.599999999999994</v>
       </c>
       <c r="G33" s="1">
-        <v>0.876</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="H33" s="1">
-        <v>0.187</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="I33" s="1">
-        <v>0.48199999999999998</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="J33" s="1">
-        <v>0.73099999999999998</v>
+        <v>0.75800000000000001</v>
       </c>
       <c r="K33" s="1">
-        <v>0.248</v>
+        <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2045,34 +2066,34 @@
         <v>13</v>
       </c>
       <c r="B34" s="1">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="C34" s="1">
-        <v>7.6719999999999997</v>
+        <v>7.3540000000000001</v>
       </c>
       <c r="D34" s="1">
-        <v>10.744999999999999</v>
+        <v>10.754</v>
       </c>
       <c r="E34" s="1">
-        <v>0.96499999999999997</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F34" s="1">
-        <v>68.72</v>
+        <v>69.819999999999993</v>
       </c>
       <c r="G34" s="1">
-        <v>0.96899999999999997</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="H34" s="1">
-        <v>-1.0999999999999999E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="I34" s="1">
-        <v>0.13200000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="J34" s="1">
-        <v>0.68300000000000005</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="K34" s="1">
-        <v>0.17199999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2080,34 +2101,34 @@
         <v>13</v>
       </c>
       <c r="B35" s="1">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="C35" s="1">
-        <v>7.6710000000000003</v>
+        <v>7.42</v>
       </c>
       <c r="D35" s="1">
-        <v>10.795999999999999</v>
+        <v>10.734999999999999</v>
       </c>
       <c r="E35" s="1">
-        <v>0.95099999999999996</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="F35" s="1">
-        <v>69.16</v>
+        <v>70.040000000000006</v>
       </c>
       <c r="G35" s="1">
-        <v>0.93400000000000005</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="H35" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="I35" s="1">
-        <v>0.217</v>
+        <v>0.36099999999999999</v>
       </c>
       <c r="J35" s="1">
-        <v>0.69099999999999995</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="K35" s="1">
-        <v>0.14399999999999999</v>
+        <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2115,34 +2136,34 @@
         <v>13</v>
       </c>
       <c r="B36" s="1">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="C36" s="1">
-        <v>7.3929999999999998</v>
+        <v>7.4450000000000003</v>
       </c>
       <c r="D36" s="1">
-        <v>10.734</v>
+        <v>10.722</v>
       </c>
       <c r="E36" s="1">
-        <v>0.93500000000000005</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="F36" s="1">
-        <v>69.599999999999994</v>
+        <v>70.260000000000005</v>
       </c>
       <c r="G36" s="1">
-        <v>0.91600000000000004</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="H36" s="1">
-        <v>8.5000000000000006E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="I36" s="1">
-        <v>0.41299999999999998</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="J36" s="1">
-        <v>0.75800000000000001</v>
+        <v>0.752</v>
       </c>
       <c r="K36" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.19500000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2150,34 +2171,34 @@
         <v>13</v>
       </c>
       <c r="B37" s="1">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="C37" s="1">
-        <v>7.3540000000000001</v>
+        <v>7.3849999999999998</v>
       </c>
       <c r="D37" s="1">
-        <v>10.754</v>
+        <v>10.714</v>
       </c>
       <c r="E37" s="1">
-        <v>0.93799999999999994</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="F37" s="1">
-        <v>69.819999999999993</v>
+        <v>70.48</v>
       </c>
       <c r="G37" s="1">
-        <v>0.93600000000000005</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="H37" s="1">
-        <v>9.5000000000000001E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="I37" s="1">
-        <v>0.32</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="J37" s="1">
-        <v>0.70899999999999996</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="K37" s="1">
-        <v>0.20499999999999999</v>
+        <v>0.19900000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2185,34 +2206,34 @@
         <v>13</v>
       </c>
       <c r="B38" s="1">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="C38" s="1">
-        <v>7.42</v>
+        <v>7.4480000000000004</v>
       </c>
       <c r="D38" s="1">
-        <v>10.734999999999999</v>
+        <v>10.715999999999999</v>
       </c>
       <c r="E38" s="1">
-        <v>0.92800000000000005</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="F38" s="1">
-        <v>70.040000000000006</v>
+        <v>70.7</v>
       </c>
       <c r="G38" s="1">
-        <v>0.92100000000000004</v>
+        <v>0.93</v>
       </c>
       <c r="H38" s="1">
-        <v>-7.0000000000000001E-3</v>
+        <v>0.105</v>
       </c>
       <c r="I38" s="1">
-        <v>0.36099999999999999</v>
+        <v>0.223</v>
       </c>
       <c r="J38" s="1">
-        <v>0.74199999999999999</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="K38" s="1">
-        <v>0.20200000000000001</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2220,34 +2241,34 @@
         <v>13</v>
       </c>
       <c r="B39" s="1">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="C39" s="1">
-        <v>7.4450000000000003</v>
+        <v>7.66</v>
       </c>
       <c r="D39" s="1">
-        <v>10.722</v>
+        <v>10.741</v>
       </c>
       <c r="E39" s="1">
-        <v>0.94099999999999995</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="F39" s="1">
-        <v>70.260000000000005</v>
+        <v>70.775000000000006</v>
       </c>
       <c r="G39" s="1">
-        <v>0.91900000000000004</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="H39" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>-3.3000000000000002E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>0.30599999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="J39" s="1">
-        <v>0.752</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="K39" s="1">
-        <v>0.19500000000000001</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2255,34 +2276,34 @@
         <v>13</v>
       </c>
       <c r="B40" s="1">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="C40" s="1">
-        <v>7.3849999999999998</v>
+        <v>7.7880000000000003</v>
       </c>
       <c r="D40" s="1">
-        <v>10.714</v>
+        <v>10.77</v>
       </c>
       <c r="E40" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="F40" s="1">
-        <v>70.48</v>
+        <v>70.849999999999994</v>
       </c>
       <c r="G40" s="1">
-        <v>0.93300000000000005</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="H40" s="1">
-        <v>-7.0000000000000001E-3</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="I40" s="1">
-        <v>0.26500000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="J40" s="1">
-        <v>0.76600000000000001</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="K40" s="1">
-        <v>0.19900000000000001</v>
+        <v>0.17599999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2290,34 +2311,34 @@
         <v>13</v>
       </c>
       <c r="B41" s="1">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="C41" s="1">
-        <v>7.4480000000000004</v>
+        <v>7.8579999999999997</v>
       </c>
       <c r="D41" s="1">
-        <v>10.715999999999999</v>
+        <v>10.78</v>
       </c>
       <c r="E41" s="1">
-        <v>0.94799999999999995</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="F41" s="1">
-        <v>70.7</v>
+        <v>70.924999999999997</v>
       </c>
       <c r="G41" s="1">
-        <v>0.93</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="H41" s="1">
-        <v>0.105</v>
+        <v>-0.13300000000000001</v>
       </c>
       <c r="I41" s="1">
-        <v>0.223</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="J41" s="1">
-        <v>0.73599999999999999</v>
+        <v>0.749</v>
       </c>
       <c r="K41" s="1">
-        <v>0.191</v>
+        <v>0.182</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2325,34 +2346,34 @@
         <v>13</v>
       </c>
       <c r="B42" s="1">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="C42" s="1">
-        <v>7.66</v>
+        <v>7.78</v>
       </c>
       <c r="D42" s="1">
-        <v>10.741</v>
+        <v>10.791</v>
       </c>
       <c r="E42" s="1">
-        <v>0.95399999999999996</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="F42" s="1">
-        <v>70.775000000000006</v>
+        <v>71</v>
       </c>
       <c r="G42" s="1">
         <v>0.94799999999999995</v>
       </c>
       <c r="H42" s="1">
-        <v>-3.3000000000000002E-2</v>
+        <v>-5.8000000000000003E-2</v>
       </c>
       <c r="I42" s="1">
-        <v>0.25</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="J42" s="1">
-        <v>0.76900000000000002</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="K42" s="1">
-        <v>0.182</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2360,34 +2381,34 @@
         <v>13</v>
       </c>
       <c r="B43" s="1">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="C43" s="1">
-        <v>7.7880000000000003</v>
+        <v>7.8890000000000002</v>
       </c>
       <c r="D43" s="1">
-        <v>10.77</v>
+        <v>10.766</v>
       </c>
       <c r="E43" s="1">
-        <v>0.96399999999999997</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="F43" s="1">
-        <v>70.849999999999994</v>
+        <v>71.075000000000003</v>
       </c>
       <c r="G43" s="1">
         <v>0.96199999999999997</v>
       </c>
       <c r="H43" s="1">
-        <v>-8.0000000000000002E-3</v>
+        <v>-0.123</v>
       </c>
       <c r="I43" s="1">
-        <v>0.192</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="J43" s="1">
-        <v>0.75600000000000001</v>
+        <v>0.748</v>
       </c>
       <c r="K43" s="1">
-        <v>0.17599999999999999</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2395,34 +2416,34 @@
         <v>13</v>
       </c>
       <c r="B44" s="1">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="C44" s="1">
-        <v>7.8579999999999997</v>
+        <v>7.7939999999999996</v>
       </c>
       <c r="D44" s="1">
-        <v>10.78</v>
+        <v>10.794</v>
       </c>
       <c r="E44" s="1">
-        <v>0.96199999999999997</v>
+        <v>0.97</v>
       </c>
       <c r="F44" s="1">
-        <v>70.924999999999997</v>
+        <v>71.150000000000006</v>
       </c>
       <c r="G44" s="1">
-        <v>0.93799999999999994</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="H44" s="1">
-        <v>-0.13300000000000001</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="I44" s="1">
-        <v>0.19900000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="J44" s="1">
-        <v>0.749</v>
+        <v>0.752</v>
       </c>
       <c r="K44" s="1">
-        <v>0.182</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2430,34 +2451,34 @@
         <v>13</v>
       </c>
       <c r="B45" s="1">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="C45" s="1">
-        <v>7.78</v>
+        <v>7.7290000000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>10.791</v>
+        <v>10.811</v>
       </c>
       <c r="E45" s="1">
-        <v>0.93700000000000006</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="F45" s="1">
-        <v>71</v>
+        <v>71.224999999999994</v>
       </c>
       <c r="G45" s="1">
-        <v>0.94799999999999995</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="H45" s="1">
-        <v>-5.8000000000000003E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="I45" s="1">
-        <v>0.19500000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="J45" s="1">
-        <v>0.73199999999999998</v>
+        <v>0.74099999999999999</v>
       </c>
       <c r="K45" s="1">
-        <v>0.18099999999999999</v>
+        <v>0.191</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -2465,138 +2486,33 @@
         <v>13</v>
       </c>
       <c r="B46" s="1">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="C46" s="1">
-        <v>7.8890000000000002</v>
+        <v>7.6989999999999998</v>
       </c>
       <c r="D46" s="1">
-        <v>10.766</v>
+        <v>10.808</v>
       </c>
       <c r="E46" s="1">
-        <v>0.96199999999999997</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="F46" s="1">
-        <v>71.075000000000003</v>
+        <v>71.3</v>
       </c>
       <c r="G46" s="1">
-        <v>0.96199999999999997</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="H46" s="1">
-        <v>-0.123</v>
+        <v>-1E-3</v>
       </c>
       <c r="I46" s="1">
-        <v>0.16400000000000001</v>
+        <v>0.185</v>
       </c>
       <c r="J46" s="1">
-        <v>0.748</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="K46" s="1">
-        <v>0.193</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="1">
-        <v>2021</v>
-      </c>
-      <c r="C47" s="1">
-        <v>7.7939999999999996</v>
-      </c>
-      <c r="D47" s="1">
-        <v>10.794</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0.97</v>
-      </c>
-      <c r="F47" s="1">
-        <v>71.150000000000006</v>
-      </c>
-      <c r="G47" s="1">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="H47" s="1">
-        <v>-3.9E-2</v>
-      </c>
-      <c r="I47" s="1">
-        <v>0.192</v>
-      </c>
-      <c r="J47" s="1">
-        <v>0.752</v>
-      </c>
-      <c r="K47" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="1">
-        <v>2022</v>
-      </c>
-      <c r="C48" s="1">
-        <v>7.7290000000000001</v>
-      </c>
-      <c r="D48" s="1">
-        <v>10.811</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0.97399999999999998</v>
-      </c>
-      <c r="F48" s="1">
-        <v>71.224999999999994</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0.95899999999999996</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="K48" s="1">
-        <v>0.191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2023</v>
-      </c>
-      <c r="C49" s="1">
-        <v>7.6989999999999998</v>
-      </c>
-      <c r="D49" s="1">
-        <v>10.808</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="F49" s="1">
-        <v>71.3</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0.94299999999999995</v>
-      </c>
-      <c r="H49" s="1">
-        <v>-1E-3</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0.185</v>
-      </c>
-      <c r="J49" s="1">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="K49" s="1">
         <v>0.17299999999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
got chart two data working
</commit_message>
<xml_diff>
--- a/data/data_chartTwo.xlsx
+++ b/data/data_chartTwo.xlsx
@@ -18,37 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
-    <t>Country name</t>
-  </si>
-  <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>Life Ladder</t>
-  </si>
-  <si>
-    <t>Log GDP per capita</t>
-  </si>
-  <si>
-    <t>Social support</t>
-  </si>
-  <si>
-    <t>Healthy life expectancy at birth</t>
-  </si>
-  <si>
-    <t>Freedom to make life choices</t>
-  </si>
-  <si>
-    <t>Generosity</t>
-  </si>
-  <si>
-    <t>Perceptions of corruption</t>
-  </si>
-  <si>
-    <t>Positive affect</t>
-  </si>
-  <si>
-    <t>Negative affect</t>
   </si>
   <si>
     <t>Afghanistan</t>
@@ -58,6 +28,36 @@
   </si>
   <si>
     <t>Finland</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ladder</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>social</t>
+  </si>
+  <si>
+    <t>lifeexp</t>
+  </si>
+  <si>
+    <t>freechoice</t>
+  </si>
+  <si>
+    <t>generosity</t>
+  </si>
+  <si>
+    <t>corruption</t>
+  </si>
+  <si>
+    <t>posaffect</t>
+  </si>
+  <si>
+    <t>negaffect</t>
   </si>
 </sst>
 </file>
@@ -897,49 +897,49 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>2008</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2009</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>2010</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
         <v>2011</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>2012</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>2013</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>2014</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>2015</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1">
         <v>2016</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1">
         <v>2017</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>2018</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1">
         <v>2019</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1">
         <v>2021</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
         <v>2022</v>
@@ -1403,8 +1403,8 @@
         <v>1.2809999999999999</v>
       </c>
       <c r="D15" s="2">
-        <f>(D17-D14)/3+D14</f>
-        <v>8.4529999999999994</v>
+        <f>D14</f>
+        <v>7.3250000000000002</v>
       </c>
       <c r="E15" s="1">
         <v>0.22800000000000001</v>
@@ -1416,8 +1416,8 @@
         <v>0.36799999999999999</v>
       </c>
       <c r="H15" s="2">
-        <f>(H17-H14)/3+H14</f>
-        <v>4.3333333333333321E-2</v>
+        <f>H14</f>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="I15" s="1">
         <v>0.73299999999999998</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1">
         <v>2023</v>
@@ -1440,8 +1440,8 @@
         <v>1.446</v>
       </c>
       <c r="D16" s="2">
-        <f>(D17-D14)*2/3+D14</f>
-        <v>9.5809999999999995</v>
+        <f>D15</f>
+        <v>7.3250000000000002</v>
       </c>
       <c r="E16" s="1">
         <v>0.36799999999999999</v>
@@ -1453,8 +1453,8 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="H16" s="2">
-        <f>(H17-H14)*2/3+H14</f>
-        <v>0.17166666666666663</v>
+        <f>H15</f>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="I16" s="1">
         <v>0.73799999999999999</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1">
         <v>2008</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1">
         <v>2010</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>2011</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>2012</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1">
         <v>2013</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B22" s="1">
         <v>2014</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1">
         <v>2015</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1">
         <v>2016</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1">
         <v>2017</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
         <v>2018</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1">
         <v>2019</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B28" s="1">
         <v>2020</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1">
         <v>2021</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B30" s="1">
         <v>2022</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B31" s="1">
         <v>2023</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1">
         <v>2008</v>
@@ -2028,7 +2028,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1">
         <v>2010</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1">
         <v>2011</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B35" s="1">
         <v>2012</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1">
         <v>2013</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B37" s="1">
         <v>2014</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1">
         <v>2015</v>
@@ -2238,7 +2238,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B39" s="1">
         <v>2016</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B40" s="1">
         <v>2017</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B41" s="1">
         <v>2018</v>
@@ -2343,7 +2343,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B42" s="1">
         <v>2019</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B43" s="1">
         <v>2020</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B44" s="1">
         <v>2021</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B45" s="1">
         <v>2022</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B46" s="1">
         <v>2023</v>

</xml_diff>

<commit_message>
Everything working except Home button.
</commit_message>
<xml_diff>
--- a/data/data_chartTwo.xlsx
+++ b/data/data_chartTwo.xlsx
@@ -897,7 +897,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,6 +2517,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C32:C46">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>